<commit_message>
change: 添加导出 json 方法
</commit_message>
<xml_diff>
--- a/battle.xlsx
+++ b/battle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiajiaju/Documents/works/git-space/ConfigMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49214C7-276B-214A-ADAA-D62A7EFD9306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6DD58D-F675-9146-A76F-9DE9CA8F4B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="21600" windowHeight="38400" xr2:uid="{69C8448C-D191-B549-9B94-DCB9C0D59B3A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{69C8448C-D191-B549-9B94-DCB9C0D59B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="说明" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
   <si>
     <t>如何配置一个 array？</t>
   </si>
@@ -298,9 +298,6 @@
     <t>每个 xlsx 只导出一个文件</t>
   </si>
   <si>
-    <t>[wave(1), wave(2), wave(3),wave(4),wave(5)]</t>
-  </si>
-  <si>
     <t>[wave(6), wave(7), wave(8)]</t>
   </si>
   <si>
@@ -310,27 +307,9 @@
     <t>[wave(40),wave(50)]</t>
   </si>
   <si>
-    <t>[wave(1), wave(1), wave(1),wave(1),wave(1)]</t>
-  </si>
-  <si>
-    <t>[wave(30), wave(2), wave(3),wave(4),wave(5)]</t>
-  </si>
-  <si>
-    <t>[wave(44), wave(2), wave(3),wave(4),wave(5)]</t>
-  </si>
-  <si>
-    <t>[wave(17), wave(2), wave(3),wave(4),wave(5)]</t>
-  </si>
-  <si>
-    <t>[group(1),group(2),group(3),group(4)]</t>
-  </si>
-  <si>
     <t>[1,2,3,4,5]</t>
   </si>
   <si>
-    <t>cell 中的内容若为 xxx(n)，代表 sheet 名为 xxx 的第 n 行</t>
-  </si>
-  <si>
     <t>3. 若数组中元素的数据类型为 object 。将字段类型标记为 array，具体数据 cell 内容为用方括号包裹并用逗号分隔的 xxx(n) 形式的内容。</t>
   </si>
   <si>
@@ -338,6 +317,21 @@
   </si>
   <si>
     <t>2. 配置一个类似 array 的 object。将字段类型标记为 object, 具体数据 cell 内容配置为该 xlsx 下某个 sheet 名。最后该 object 为以某个 sheet 的每行为一个 value，每行第一列的数据为 key 的 object。</t>
+  </si>
+  <si>
+    <t>cell 中的内容若为 xxx(n)，代表 sheet 名为 xxx 的第 n 行（excel 中的行号）</t>
+  </si>
+  <si>
+    <t>[wave(4), wave(5), wave(6),wave(7),wave(8)]</t>
+  </si>
+  <si>
+    <t>[wave(4), wave(4), wave(5),wave(6),wave(7)]</t>
+  </si>
+  <si>
+    <t>[wave(30), wave(23), wave(4),wave(46),wave(44)]</t>
+  </si>
+  <si>
+    <t>[group(4),group(5),group(6),group(7)]</t>
   </si>
 </sst>
 </file>
@@ -713,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9B63AC-0B3B-2640-B5D2-67834016F592}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -764,7 +758,7 @@
     </row>
     <row r="9" spans="1:1" ht="24">
       <c r="A9" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="24">
@@ -789,7 +783,7 @@
     </row>
     <row r="20" spans="1:1" s="1" customFormat="1" ht="25" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:1" s="1" customFormat="1" ht="25" customHeight="1">
@@ -799,12 +793,12 @@
     </row>
     <row r="26" spans="1:1" s="1" customFormat="1" ht="25" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:1" s="1" customFormat="1" ht="25" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -817,7 +811,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -927,7 +921,7 @@
         <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -953,7 +947,7 @@
         <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -973,7 +967,7 @@
         <v>73</v>
       </c>
       <c r="H6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -999,7 +993,7 @@
         <v>74</v>
       </c>
       <c r="H7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1071,7 +1065,7 @@
         <v>77</v>
       </c>
       <c r="H10" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1097,7 +1091,7 @@
         <v>78</v>
       </c>
       <c r="H11" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1123,7 +1117,7 @@
         <v>79</v>
       </c>
       <c r="H12" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1149,7 +1143,7 @@
         <v>80</v>
       </c>
       <c r="H13" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1162,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C501EE-98C5-7248-BA65-A78ABE9029E9}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1200,7 +1194,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1208,7 +1202,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1216,7 +1210,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1224,7 +1218,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1232,7 +1226,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1240,7 +1234,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1248,7 +1242,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1256,7 +1250,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1264,7 +1258,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1272,7 +1266,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1280,7 +1274,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1288,7 +1282,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1296,7 +1290,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1304,7 +1298,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1312,7 +1306,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1320,7 +1314,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1328,7 +1322,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1336,7 +1330,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1344,7 +1338,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1352,7 +1346,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1360,7 +1354,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1368,7 +1362,7 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1376,7 +1370,7 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1384,7 +1378,7 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1392,7 +1386,7 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1400,7 +1394,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1408,7 +1402,7 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1416,7 +1410,7 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1424,7 +1418,7 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1432,7 +1426,7 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1440,7 +1434,7 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1448,7 +1442,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1456,7 +1450,7 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1464,7 +1458,7 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1472,7 +1466,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1480,7 +1474,7 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1488,7 +1482,7 @@
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1496,7 +1490,7 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1504,7 +1498,7 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1512,7 +1506,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1520,7 +1514,7 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1528,7 +1522,7 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1536,7 +1530,7 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1544,7 +1538,7 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1552,7 +1546,7 @@
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1560,7 +1554,7 @@
         <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1568,7 +1562,7 @@
         <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1576,7 +1570,7 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1584,7 +1578,7 @@
         <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1592,7 +1586,7 @@
         <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1639,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1647,7 +1641,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1655,7 +1649,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1663,7 +1657,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1675,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014E316E-A825-2049-9EF4-9C813102BEB0}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>